<commit_message>
feat: backend fully functional and tested
</commit_message>
<xml_diff>
--- a/backend/testeclientes.xlsx
+++ b/backend/testeclientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbasb\Documents\Estudos\swing-trade-basket-generator\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81575EDF-19BA-4FEE-B790-F46940836B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9964F0DA-D582-4F08-8385-8E597CFD2237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C1C674A6-FDFC-41A8-AA21-AC1EBC25BAD4}"/>
   </bookViews>
@@ -37,30 +37,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="54">
-  <si>
-    <t>Conta</t>
-  </si>
-  <si>
-    <t>Assessor RV</t>
-  </si>
-  <si>
-    <t>Advisor</t>
-  </si>
-  <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <t>Estratégia</t>
-  </si>
-  <si>
-    <t>Net Total</t>
-  </si>
-  <si>
-    <t>Net Disponível</t>
-  </si>
-  <si>
-    <t>Valor Médio por Operação</t>
-  </si>
   <si>
     <t>Breno</t>
   </si>
@@ -198,6 +174,30 @@
   </si>
   <si>
     <t>Fernando</t>
+  </si>
+  <si>
+    <t>NUMERO CONTA</t>
+  </si>
+  <si>
+    <t>ASSESSOR RV</t>
+  </si>
+  <si>
+    <t>ADVISOR</t>
+  </si>
+  <si>
+    <t>CLIENTE</t>
+  </si>
+  <si>
+    <t>ESTRATÉGIA</t>
+  </si>
+  <si>
+    <t>NET TOTAL</t>
+  </si>
+  <si>
+    <t>NET DISPONÍVEL</t>
+  </si>
+  <si>
+    <t>VALOR MEDIO POR OPERAÇÃO</t>
   </si>
 </sst>
 </file>
@@ -684,45 +684,45 @@
   <dimension ref="A1:X940"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="66" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B19"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -746,16 +746,16 @@
         <v>8001</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F2" s="4">
         <v>33000</v>
@@ -788,16 +788,16 @@
         <v>8002</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F3" s="4">
         <v>48000</v>
@@ -830,16 +830,16 @@
         <v>8003</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F4" s="4">
         <v>80000</v>
@@ -872,16 +872,16 @@
         <v>8004</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F5" s="4">
         <v>50000</v>
@@ -914,16 +914,16 @@
         <v>8005</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F6" s="4">
         <v>50000</v>
@@ -956,16 +956,16 @@
         <v>8006</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F7" s="4">
         <v>50000</v>
@@ -998,16 +998,16 @@
         <v>8007</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F8" s="4">
         <v>50000</v>
@@ -1040,16 +1040,16 @@
         <v>8008</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4">
         <v>50000</v>
@@ -1082,16 +1082,16 @@
         <v>8009</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F10" s="4">
         <v>50000</v>
@@ -1124,16 +1124,16 @@
         <v>8010</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F11" s="4">
         <v>50000</v>
@@ -1166,16 +1166,16 @@
         <v>8011</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F12" s="4">
         <v>50000</v>
@@ -1208,16 +1208,16 @@
         <v>8012</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F13" s="4">
         <v>50000</v>
@@ -1250,16 +1250,16 @@
         <v>8013</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F14" s="4">
         <v>50000</v>
@@ -1292,16 +1292,16 @@
         <v>8014</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F15" s="4">
         <v>50000</v>
@@ -1334,16 +1334,16 @@
         <v>8015</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F16" s="4">
         <v>50000</v>
@@ -1376,16 +1376,16 @@
         <v>8016</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F17" s="4">
         <v>50000</v>
@@ -1418,16 +1418,16 @@
         <v>8017</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F18" s="4">
         <v>50000</v>
@@ -1460,16 +1460,16 @@
         <v>8018</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F19" s="4">
         <v>35000</v>
@@ -1502,16 +1502,16 @@
         <v>8019</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F20" s="4">
         <v>52000</v>
@@ -1544,16 +1544,16 @@
         <v>8020</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F21" s="4">
         <v>100000</v>
@@ -1586,16 +1586,16 @@
         <v>8021</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F22" s="4">
         <v>100000</v>
@@ -1628,16 +1628,16 @@
         <v>8022</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F23" s="4">
         <v>100000</v>
@@ -1670,16 +1670,16 @@
         <v>8023</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F24" s="4">
         <v>100000</v>
@@ -1712,16 +1712,16 @@
         <v>8024</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F25" s="4">
         <v>70000</v>
@@ -1754,16 +1754,16 @@
         <v>8025</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F26" s="4">
         <v>24000</v>
@@ -1796,16 +1796,16 @@
         <v>8026</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F27" s="4">
         <v>40000</v>
@@ -1838,16 +1838,16 @@
         <v>8027</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F28" s="4">
         <v>150000</v>
@@ -1880,16 +1880,16 @@
         <v>8028</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F29" s="4">
         <v>25000</v>
@@ -1922,16 +1922,16 @@
         <v>8029</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F30" s="4">
         <v>150000</v>
@@ -1964,16 +1964,16 @@
         <v>8030</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F31" s="4">
         <v>40000</v>
@@ -2006,16 +2006,16 @@
         <v>8031</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F32" s="4">
         <v>45000</v>
@@ -2048,16 +2048,16 @@
         <v>8032</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F33" s="4">
         <v>90000</v>
@@ -2090,16 +2090,16 @@
         <v>8033</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F34" s="4">
         <v>60000</v>
@@ -2132,16 +2132,16 @@
         <v>8034</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F35" s="4">
         <v>30000</v>
@@ -2174,16 +2174,16 @@
         <v>8035</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F36" s="4">
         <v>300000</v>
@@ -2216,16 +2216,16 @@
         <v>8036</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F37" s="4">
         <v>43000</v>
@@ -2258,16 +2258,16 @@
         <v>8037</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F38" s="4">
         <v>50000</v>
@@ -2300,16 +2300,16 @@
         <v>8038</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F39" s="4">
         <v>50000</v>
@@ -2342,16 +2342,16 @@
         <v>8039</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F40" s="4">
         <v>100000</v>
@@ -2384,16 +2384,16 @@
         <v>8040</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F41" s="4">
         <v>100000</v>
@@ -25797,5 +25797,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>